<commit_message>
Program now reads the incidence matrix and the scores difference. Returns in a pair.
</commit_message>
<xml_diff>
--- a/swiss_draw.xlsx
+++ b/swiss_draw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="swiss_matches" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>Cosmo</t>
-  </si>
-  <si>
-    <t>ND Krsko</t>
   </si>
   <si>
     <t>Vertigo</t>
@@ -30,25 +27,7 @@
     <t>Frizmi</t>
   </si>
   <si>
-    <t>team1</t>
-  </si>
-  <si>
-    <t>team2</t>
-  </si>
-  <si>
-    <t>Rubber Duckies</t>
-  </si>
-  <si>
-    <t>Druga 1</t>
-  </si>
-  <si>
-    <t>Tretja 2</t>
-  </si>
-  <si>
-    <t>SŠSB 1</t>
-  </si>
-  <si>
-    <t>II. Druga</t>
+    <t>Nuclear Discs</t>
   </si>
 </sst>
 </file>
@@ -381,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -395,18 +374,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>15</v>
+      </c>
+      <c r="D1">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -420,54 +405,27 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>15</v>
       </c>
-      <c r="D3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="str">
-        <f>A2</f>
-        <v>Cosmo</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D4">
         <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -478,10 +436,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,17 +459,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working calculator with and example in Swiss.py. Moved some code around.
</commit_message>
<xml_diff>
--- a/swiss_draw.xlsx
+++ b/swiss_draw.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Cosmo</t>
   </si>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -377,55 +377,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1">
         <v>15</v>
       </c>
       <c r="D1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
         <v>15</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic team matchups added
</commit_message>
<xml_diff>
--- a/swiss_draw.xlsx
+++ b/swiss_draw.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
-  <si>
-    <t>Cosmo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Vertigo</t>
   </si>
@@ -28,6 +25,9 @@
   </si>
   <si>
     <t>Nuclear Discs</t>
+  </si>
+  <si>
+    <t>Cosmoo</t>
   </si>
 </sst>
 </file>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -374,10 +374,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>15</v>
@@ -391,27 +391,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -435,22 +421,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imporvement in Gauss and system. Works, but not ideal. If there are not enough matches, the system doesn't do a good enough job of calculating the scores. It isn't fair. TODO
</commit_message>
<xml_diff>
--- a/swiss_draw.xlsx
+++ b/swiss_draw.xlsx
@@ -10,31 +10,81 @@
     <sheet name="swiss_matches" sheetId="1" r:id="rId1"/>
     <sheet name="teams" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
+    <sheet name="List1" sheetId="4" r:id="rId4"/>
+    <sheet name="List2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
-  <si>
-    <t>Vertigo</t>
-  </si>
-  <si>
-    <t>Frizmi</t>
-  </si>
-  <si>
-    <t>Nuclear Discs</t>
-  </si>
-  <si>
-    <t>Cosmoo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="20">
+  <si>
+    <t>Chaos Ultimate</t>
+  </si>
+  <si>
+    <t>Triple Mamasitas</t>
+  </si>
+  <si>
+    <t>+ Update Score</t>
+  </si>
+  <si>
+    <t>Helsinki Ultimate Team</t>
+  </si>
+  <si>
+    <t>Ultimate Dragons</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t>Enraladas</t>
+  </si>
+  <si>
+    <t>Gentleladies</t>
+  </si>
+  <si>
+    <t>Slovak women national team</t>
+  </si>
+  <si>
+    <t>Mainzelmädchen</t>
+  </si>
+  <si>
+    <t>Southwest</t>
+  </si>
+  <si>
+    <t>Flying Angels Berne - FABulous</t>
+  </si>
+  <si>
+    <t>Dublin Gravity</t>
+  </si>
+  <si>
+    <t>Atletico</t>
+  </si>
+  <si>
+    <t>Troubles</t>
+  </si>
+  <si>
+    <t>YAKA</t>
+  </si>
+  <si>
+    <t>Czech Women</t>
+  </si>
+  <si>
+    <t>Friday, 12:30pm </t>
+  </si>
+  <si>
+    <t>13 - 14</t>
+  </si>
+  <si>
+    <t>Field 5 - Livestream</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,16 +93,51 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -60,14 +145,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperpovezava" xfId="1" builtinId="8"/>
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -374,13 +512,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D1">
         <v>10</v>
@@ -388,16 +526,324 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
-        <v>10</v>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -408,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,22 +867,82 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -447,6 +953,583 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="39" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" ht="39" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" ht="39" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" ht="44.25" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" ht="39" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:2" ht="44.25" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" ht="39" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="11">
+        <v>43262</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="11">
+        <v>43235</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="11">
+        <v>43388</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12">
+        <v>42064</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="11">
+        <v>43234</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12">
+        <v>42248</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="12">
+        <v>41883</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1" display="https://www.leaguevine.com/teams/33359/yaka/"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="A1:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>9</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -454,6 +1537,5 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The scoring is now fair and disjunct groups get the absolute value of the sum of their scores minimised.
</commit_message>
<xml_diff>
--- a/swiss_draw.xlsx
+++ b/swiss_draw.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="20">
   <si>
     <t>Chaos Ultimate</t>
   </si>
@@ -177,18 +177,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -203,6 +191,18 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperpovezava" xfId="1" builtinId="8"/>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="A9:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,230 +620,6 @@
       </c>
       <c r="D8">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>15</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21">
-        <v>9</v>
-      </c>
-      <c r="D21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22">
-        <v>15</v>
-      </c>
-      <c r="D22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>15</v>
-      </c>
-      <c r="D23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -974,104 +750,104 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="39" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" ht="39" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" ht="39" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="44.25" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" ht="39" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" ht="44.25" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" ht="39" customHeight="1">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="10"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="7">
         <v>43262</v>
       </c>
       <c r="C21" t="s">
@@ -1088,7 +864,7 @@
       <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="7">
         <v>43235</v>
       </c>
       <c r="C22" t="s">
@@ -1105,7 +881,7 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="7">
         <v>43388</v>
       </c>
       <c r="C23" t="s">
@@ -1122,7 +898,7 @@
       <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="8">
         <v>42064</v>
       </c>
       <c r="C24" t="s">
@@ -1139,7 +915,7 @@
       <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="7">
         <v>43234</v>
       </c>
       <c r="C25" t="s">
@@ -1173,7 +949,7 @@
       <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="8">
         <v>42248</v>
       </c>
       <c r="C27" t="s">
@@ -1190,7 +966,7 @@
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="8">
         <v>41883</v>
       </c>
       <c r="C28" t="s">
@@ -1287,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="A1:D16"/>
+      <selection activeCell="D24" sqref="A1:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1521,6 +1297,118 @@
       </c>
       <c r="D16">
         <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>